<commit_message>
In this new version we rewrite something functions
</commit_message>
<xml_diff>
--- a/results_alignment.xlsx
+++ b/results_alignment.xlsx
@@ -433,7 +433,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>-132.4921844903147</v>
+        <v>-132.5699477100279</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -444,7 +444,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>-396.975216871399</v>
+        <v>-396.747853794243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>